<commit_message>
home commit 30 July lots of changes
</commit_message>
<xml_diff>
--- a/LOGS/0b15b63c-f228-489f-9e22-a84e8d3ce36f/main_page_service_output/notes_standard_cropped_df.xlsx
+++ b/LOGS/0b15b63c-f228-489f-9e22-a84e8d3ce36f/main_page_service_output/notes_standard_cropped_df.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="137">
   <si>
     <t>line_item_0</t>
   </si>
@@ -75,6 +75,9 @@
     <t>Related party receivables (Note 20)</t>
   </si>
   <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>Raw materials</t>
   </si>
   <si>
@@ -106,9 +109,6 @@
   </si>
   <si>
     <t>Other related parties</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>Ultimate parent</t>
@@ -1494,7 +1494,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -2916,7 +2916,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -4005,6 +4005,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
       <c r="C5">
         <v>29557</v>
       </c>
@@ -4020,7 +4023,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>25662</v>
@@ -4037,7 +4040,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>3895</v>
@@ -4213,6 +4216,9 @@
       </c>
     </row>
     <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
       <c r="B5" t="s">
         <v>118</v>
       </c>
@@ -4230,6 +4236,9 @@
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
       <c r="B6" t="s">
         <v>118</v>
       </c>
@@ -4307,6 +4316,9 @@
       </c>
     </row>
     <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
       <c r="B10" t="s">
         <v>119</v>
       </c>
@@ -4324,6 +4336,9 @@
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
       <c r="B11" t="s">
         <v>119</v>
       </c>
@@ -4381,6 +4396,9 @@
       </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
       <c r="B14" t="s">
         <v>120</v>
       </c>
@@ -4398,6 +4416,9 @@
       </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
       <c r="B15" t="s">
         <v>120</v>
       </c>
@@ -4419,7 +4440,7 @@
         <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>35790</v>
@@ -4439,7 +4460,7 @@
         <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C17">
         <v>-40046</v>
@@ -4459,7 +4480,7 @@
         <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <v>-4256</v>
@@ -4535,6 +4556,9 @@
       </c>
     </row>
     <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
       <c r="B22" t="s">
         <v>118</v>
       </c>
@@ -4552,6 +4576,9 @@
       </c>
     </row>
     <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
       <c r="B23" t="s">
         <v>118</v>
       </c>
@@ -4629,6 +4656,9 @@
       </c>
     </row>
     <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
       <c r="B27" t="s">
         <v>119</v>
       </c>
@@ -4646,6 +4676,9 @@
       </c>
     </row>
     <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
       <c r="B28" t="s">
         <v>119</v>
       </c>
@@ -4703,6 +4736,9 @@
       </c>
     </row>
     <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
       <c r="B31" t="s">
         <v>120</v>
       </c>
@@ -4720,6 +4756,9 @@
       </c>
     </row>
     <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
       <c r="B32" t="s">
         <v>120</v>
       </c>
@@ -4741,7 +4780,7 @@
         <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C33">
         <v>44822</v>
@@ -4761,7 +4800,7 @@
         <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <v>-9032</v>
@@ -4781,7 +4820,7 @@
         <v>97</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C35">
         <v>35790</v>
@@ -4864,6 +4903,9 @@
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
       <c r="C4">
         <v>13624</v>
       </c>
@@ -4912,6 +4954,9 @@
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
       <c r="C7">
         <v>11999</v>
       </c>
@@ -5407,6 +5452,9 @@
       </c>
     </row>
     <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
       <c r="C6">
         <v>13631</v>
       </c>
@@ -5489,6 +5537,9 @@
       </c>
     </row>
     <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
       <c r="C11">
         <v>10144</v>
       </c>
@@ -5637,6 +5688,9 @@
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
       <c r="C4">
         <v>-539</v>
       </c>
@@ -5685,6 +5739,9 @@
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
       <c r="C7">
         <v>-618</v>
       </c>
@@ -5733,7 +5790,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>18547</v>
@@ -5750,7 +5807,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>8651</v>
@@ -5766,6 +5823,9 @@
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
       <c r="C4">
         <v>27198</v>
       </c>
@@ -5781,7 +5841,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>19816</v>
@@ -5798,7 +5858,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>7137</v>
@@ -5814,6 +5874,9 @@
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
       <c r="C7">
         <v>26953</v>
       </c>
@@ -5862,10 +5925,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -5882,10 +5945,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -5901,8 +5964,11 @@
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5919,10 +5985,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5939,10 +6005,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>51</v>
@@ -5959,10 +6025,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>29702</v>
@@ -5978,8 +6044,11 @@
       </c>
     </row>
     <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>29753</v>
@@ -5996,10 +6065,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>12453</v>
@@ -6044,18 +6113,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -6081,7 +6150,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -6107,7 +6176,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -6133,7 +6202,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>24</v>
@@ -6159,7 +6228,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
@@ -6185,7 +6254,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -6211,7 +6280,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -6237,7 +6306,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
@@ -6263,7 +6332,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -6289,7 +6358,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
@@ -6315,7 +6384,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -6341,7 +6410,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -6367,7 +6436,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -6393,7 +6462,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
@@ -6419,7 +6488,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
@@ -6445,7 +6514,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
@@ -6471,7 +6540,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
@@ -6497,7 +6566,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
@@ -6554,7 +6623,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -7907,7 +7976,7 @@
         <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F50">
         <v>2020</v>
@@ -7927,7 +7996,7 @@
         <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F51">
         <v>2020</v>
@@ -7947,7 +8016,7 @@
         <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F52">
         <v>2020</v>
@@ -7967,7 +8036,7 @@
         <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F53">
         <v>2020</v>
@@ -7987,7 +8056,7 @@
         <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F54">
         <v>2020</v>
@@ -8007,7 +8076,7 @@
         <v>7</v>
       </c>
       <c r="E55" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F55">
         <v>2020</v>
@@ -8027,7 +8096,7 @@
         <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F56">
         <v>2020</v>
@@ -8047,7 +8116,7 @@
         <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F57">
         <v>2020</v>
@@ -8067,7 +8136,7 @@
         <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F58">
         <v>2020</v>
@@ -8087,7 +8156,7 @@
         <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F59">
         <v>2020</v>
@@ -8107,7 +8176,7 @@
         <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F60">
         <v>2020</v>
@@ -8127,7 +8196,7 @@
         <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F61">
         <v>2019</v>

</xml_diff>